<commit_message>
updated cn_authorization, changed setOwner to operate on a single object (revisit lists in general later)
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26360" yWindow="-700" windowWidth="24060" windowHeight="17400" tabRatio="500"/>
+    <workbookView xWindow="-28460" yWindow="-1180" windowWidth="26660" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>token, GUID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,6 +66,82 @@
   </si>
   <si>
     <t>Use Cases</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REST path</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_authorization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>setAccess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>setOwner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>newAccount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>verifyToken</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user, password, [authSystem]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AuthToken</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvalidCredentials</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AuthenticationTimeout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID, accessLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, userid, GUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidtoken</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>username, password, authSystem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrincipalType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierNotUnique</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -604,373 +680,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="H25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="H27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="H33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="26">
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="H36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="26">
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="H38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="H39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="C42" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="H43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="C44" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="H45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="H46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="H48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="G14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="G18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="G22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="G23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="G25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="G27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="G28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="G30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="G32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7">
-      <c r="G33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" ht="26">
-      <c r="C34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7">
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7">
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" ht="26">
-      <c r="C37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7">
-      <c r="G38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7">
-      <c r="G39" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Syncing images, a few minor edits
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28460" yWindow="-1180" windowWidth="26660" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="-28440" yWindow="-780" windowWidth="26660" windowHeight="17380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MethodMadnessMap" sheetId="1" r:id="rId1"/>
+    <sheet name="RequirementsUsecaseMap" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ObjectList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to work on query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to work on query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_replication</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_register</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_health</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_synchronization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_authorization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_replication</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_capabilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_health</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID, operation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC37</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /mn/object/&lt;guid&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /mn/object/&lt;guid&gt;/meta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /cn/object/&lt;guid&gt;/meta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /cn/object/&lt;guid&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>listObjects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /mn/object/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ObjectList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>token, GUID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -142,6 +263,10 @@
   </si>
   <si>
     <t>IdentifierNotUnique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -680,19 +805,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
@@ -700,442 +826,593 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="H3" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="H5" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="H6" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="H7" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="H8" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="C9" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="H10" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="H11" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="H12" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="H13" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="H14" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="C15" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="H16" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="C17" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="H18" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="C19" t="s">
-        <v>44</v>
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="H20" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="C21" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="H22" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="2:8">
       <c r="H23" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="C24" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="H25" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="H28" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" t="s">
-        <v>57</v>
+      <c r="B29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="H30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>57</v>
+      <c r="B30" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:8">
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>85</v>
+      </c>
       <c r="H32" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="H33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="26">
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
       <c r="H34" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="2:8">
       <c r="C35" t="s">
-        <v>69</v>
+        <v>97</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G35" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:8">
       <c r="H36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="26">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
       <c r="C37" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:8">
       <c r="H38" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="2:8">
       <c r="H39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="26">
       <c r="C40" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:8">
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>35</v>
+      </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="2:8">
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" t="s">
-        <v>6</v>
-      </c>
       <c r="H42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="26">
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" t="s">
+        <v>36</v>
+      </c>
       <c r="H43" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="2:8">
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" t="s">
-        <v>26</v>
-      </c>
       <c r="H44" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="2:8">
       <c r="H45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="H47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="H49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" t="s">
+        <v>56</v>
+      </c>
+      <c r="H50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="H51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="H52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="H46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="C47" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="H48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" t="s">
+      <c r="G53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="H54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="C55" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G55" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="C56" t="s">
         <v>18</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H57" t="s">
+        <v>88</v>
+      </c>
+      <c r="J57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="H58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="C59" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>87</v>
+      </c>
+      <c r="H59" t="s">
+        <v>88</v>
+      </c>
+      <c r="J59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="H60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1149,4 +1426,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Set exception detail codes for currently defined functions.  Closing #469
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28440" yWindow="-780" windowWidth="26660" windowHeight="17380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3240" yWindow="-420" windowWidth="24960" windowHeight="20380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MethodMadnessMap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="112">
+  <si>
+    <t>Consistent mechanism for identifying users</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>typeOfOperation, targetGUID, requestorIdentity, dateOfRequest, ...</t>
+  </si>
+  <si>
+    <t>Recast parameters as query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>NotAuthorized</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -142,6 +157,26 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Requirement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Identifiers for all objects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support Data Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Efficient mechanisms for users to discover content</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support arbitrary unique identifiers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>token, GUID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -370,6 +405,9 @@
   <si>
     <t>LogRecords</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
   </si>
   <si>
     <t>NotAuthorized</t>
@@ -467,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,6 +513,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,11 +846,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -817,606 +858,804 @@
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="26">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="26">
       <c r="B2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="H3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>99</v>
+      </c>
+      <c r="I3">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="26">
       <c r="C4" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="I4">
+        <v>1040</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="H5" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="I5">
+        <v>1060</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="H6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>46</v>
+      </c>
+      <c r="I6">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="26">
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="I7">
+        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="H8" t="s">
-        <v>93</v>
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>1120</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" t="s">
-        <v>82</v>
-      </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>101</v>
+      </c>
+      <c r="I9">
+        <v>1140</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="H10" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="I10">
+        <v>1160</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="H11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="26">
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
       <c r="H12" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="I12">
+        <v>1200</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="H13" t="s">
-        <v>89</v>
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>1220</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="H14" t="s">
-        <v>93</v>
+        <v>101</v>
+      </c>
+      <c r="I14">
+        <v>1240</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" t="s">
-        <v>82</v>
-      </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>102</v>
+      </c>
+      <c r="I15">
+        <v>1260</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="H16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="H17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="26">
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="26">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="H21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="65">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="H23" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="H24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="39">
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="H18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="H20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="H22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="H23" t="s">
+      <c r="G25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25">
+        <v>1460</v>
+      </c>
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="H26" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="104">
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="26">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="H29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="26">
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="26">
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="H25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="H28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>85</v>
-      </c>
-      <c r="H32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="H33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="H34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="C35" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
       <c r="H36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="C37" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" t="s">
-        <v>34</v>
-      </c>
+      <c r="I36">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
       <c r="H37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8">
+        <v>99</v>
+      </c>
+      <c r="I37">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
       <c r="H38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8">
+        <v>104</v>
+      </c>
+      <c r="I38">
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="130">
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="H39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="26">
+        <v>47</v>
+      </c>
+      <c r="I39">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="26">
       <c r="C40" t="s">
+        <v>108</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="H41" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="C41" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8">
+      <c r="I41">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
       <c r="H42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="26">
+        <v>46</v>
+      </c>
+      <c r="I42">
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="39">
       <c r="C43" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G43" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8">
+        <v>98</v>
+      </c>
+      <c r="I43">
+        <v>4180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
       <c r="H44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
+        <v>46</v>
+      </c>
+      <c r="I44">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="91">
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" t="s">
+        <v>45</v>
+      </c>
       <c r="H45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" t="s">
-        <v>50</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I45">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
       <c r="H46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8">
+        <v>99</v>
+      </c>
+      <c r="I46">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
       <c r="H47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8">
+        <v>48</v>
+      </c>
+      <c r="I47">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="26">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>54</v>
+        <v>98</v>
+      </c>
+      <c r="I48">
+        <v>4280</v>
+      </c>
+      <c r="J48" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="2:10">
       <c r="H49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10">
+        <v>46</v>
+      </c>
+      <c r="I49">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="26">
       <c r="C50" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="H50" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="I50">
+        <v>4320</v>
+      </c>
+      <c r="J50" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="2:10">
       <c r="H51" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10">
+        <v>46</v>
+      </c>
+      <c r="I51">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="52">
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" t="s">
+        <v>59</v>
+      </c>
       <c r="H52" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="I52">
+        <v>4360</v>
       </c>
     </row>
     <row r="53" spans="2:10">
-      <c r="C53" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G53" t="s">
-        <v>59</v>
-      </c>
       <c r="H53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10">
+        <v>61</v>
+      </c>
+      <c r="I53">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="52">
+      <c r="C54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" t="s">
+        <v>45</v>
+      </c>
       <c r="H54" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+      <c r="I54">
+        <v>4400</v>
       </c>
     </row>
     <row r="55" spans="2:10">
-      <c r="C55" t="s">
-        <v>48</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G55" t="s">
-        <v>36</v>
-      </c>
       <c r="H55" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10">
+        <v>99</v>
+      </c>
+      <c r="I55">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="39">
       <c r="C56" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="G56" t="s">
-        <v>36</v>
+        <v>65</v>
+      </c>
+      <c r="H56" t="s">
+        <v>98</v>
+      </c>
+      <c r="I56">
+        <v>4440</v>
       </c>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G57" t="s">
-        <v>4</v>
-      </c>
       <c r="H57" t="s">
-        <v>88</v>
-      </c>
-      <c r="J57" t="s">
-        <v>5</v>
+        <v>99</v>
+      </c>
+      <c r="I57">
+        <v>4460</v>
       </c>
     </row>
     <row r="58" spans="2:10">
       <c r="H58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10">
+        <v>66</v>
+      </c>
+      <c r="I58">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="65">
       <c r="C59" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="G59" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="H59" t="s">
-        <v>88</v>
-      </c>
-      <c r="J59" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="I59">
+        <v>4500</v>
       </c>
     </row>
     <row r="60" spans="2:10">
       <c r="H60" t="s">
-        <v>37</v>
+        <v>60</v>
+      </c>
+      <c r="I60">
+        <v>4520</v>
       </c>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10">
-      <c r="B62" t="s">
-        <v>11</v>
+      <c r="C61" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G61" t="s">
+        <v>45</v>
+      </c>
+      <c r="H61" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" ht="39">
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>45</v>
+      </c>
+      <c r="H62" t="s">
+        <v>99</v>
+      </c>
+      <c r="I62">
+        <v>4560</v>
       </c>
     </row>
     <row r="63" spans="2:10">
       <c r="B63" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="H63" t="s">
+        <v>97</v>
+      </c>
+      <c r="I63">
+        <v>4580</v>
       </c>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1430,13 +1669,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
+  <cols>
+    <col min="1" max="1" width="12" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4">
+        <v>317</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4">
+        <v>317.31799999999998</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4">
+        <v>383</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4">
+        <v>384</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4">
+        <v>390</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Removed non-sensical InvalidRequest from CN_crud.resolve, updated REST interface for resolve
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="480" windowWidth="26340" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="-100" windowWidth="26340" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MethodMadnessMap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
   <si>
     <t>NotFound</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -38,91 +38,87 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>getSystemMetadata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>API Doc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Types</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REST Doc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotImplemented</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, startTime, [endTime], [replicaStatus], [start], [count]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>resolve</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC06, UC09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierNotUnique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUID, systemMetadata, scienceMetadata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserveIdentifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC04, UC38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getLogRecords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC33</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>listObjects</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>getSystemMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>get</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>API Doc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Types</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REST Doc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NotImplemented</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, startTime, [endTime], [replicaStatus], [start], [count]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getSystemMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>search</t>
+    <t>NA</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>create</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>resolve</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC06, UC09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, GUID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierNotUnique</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GUID, systemMetadata, scienceMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>reserveIdentifier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC04, UC38</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getLogRecords</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC33</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -591,7 +587,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="57"/>
+      <color indexed="17"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -628,10 +624,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,7 +961,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -984,75 +980,75 @@
   <sheetData>
     <row r="1" spans="1:13" ht="61">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L2">
         <v>1000</v>
@@ -1060,37 +1056,39 @@
     </row>
     <row r="3" spans="1:13">
       <c r="K3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L3">
         <v>1020</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5"/>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
       <c r="G4" t="s">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L4">
         <v>1040</v>
@@ -1098,7 +1096,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="K5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L5">
         <v>1060</v>
@@ -1106,7 +1104,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="K6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L6">
         <v>1080</v>
@@ -1114,19 +1112,19 @@
     </row>
     <row r="7" spans="1:13">
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L7">
         <v>1100</v>
@@ -1134,7 +1132,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="K8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L8">
         <v>1120</v>
@@ -1142,7 +1140,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="K9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L9">
         <v>1140</v>
@@ -1150,7 +1148,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="K10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L10">
         <v>1160</v>
@@ -1158,7 +1156,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="K11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L11">
         <v>1180</v>
@@ -1166,16 +1164,16 @@
     </row>
     <row r="12" spans="1:13">
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L12">
         <v>1200</v>
@@ -1183,7 +1181,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="K13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L13">
         <v>1220</v>
@@ -1191,7 +1189,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="K14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L14">
         <v>1240</v>
@@ -1199,7 +1197,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="K15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L15">
         <v>1260</v>
@@ -1207,7 +1205,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="K16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L16">
         <v>1280</v>
@@ -1215,7 +1213,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="K17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L17">
         <v>1300</v>
@@ -1223,16 +1221,16 @@
     </row>
     <row r="18" spans="2:13">
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L18">
         <v>1320</v>
@@ -1240,7 +1238,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="K19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L19">
         <v>1340</v>
@@ -1248,16 +1246,16 @@
     </row>
     <row r="20" spans="2:13">
       <c r="C20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L20">
         <v>1360</v>
@@ -1265,7 +1263,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="K21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L21">
         <v>1380</v>
@@ -1273,16 +1271,16 @@
     </row>
     <row r="22" spans="2:13" ht="26">
       <c r="C22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L22">
         <v>1400</v>
@@ -1290,7 +1288,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="K23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L23">
         <v>1420</v>
@@ -1298,7 +1296,7 @@
     </row>
     <row r="24" spans="2:13">
       <c r="K24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L24">
         <v>1440</v>
@@ -1306,27 +1304,27 @@
     </row>
     <row r="25" spans="2:13" ht="26">
       <c r="C25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L25">
         <v>1460</v>
       </c>
       <c r="M25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="2:13">
       <c r="K26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L26">
         <v>1480</v>
@@ -1334,16 +1332,16 @@
     </row>
     <row r="27" spans="2:13" ht="52">
       <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G27" t="s">
-        <v>71</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="K27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L27">
         <v>1500</v>
@@ -1351,32 +1349,34 @@
     </row>
     <row r="28" spans="2:13" ht="52">
       <c r="B28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5">
-        <v>1</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
       <c r="G28" t="s">
         <v>3</v>
       </c>
       <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>34</v>
-      </c>
-      <c r="K28" t="s">
-        <v>35</v>
       </c>
       <c r="L28">
         <v>1520</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="K29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L29">
         <v>1540</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="30" spans="2:13">
       <c r="K30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L30">
         <v>1560</v>
@@ -1400,25 +1400,25 @@
     </row>
     <row r="31" spans="2:13">
       <c r="C31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:12">
       <c r="B33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="2:12">
       <c r="B34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="2:12">
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K35" t="s">
         <v>0</v>
@@ -1426,31 +1426,34 @@
     </row>
     <row r="39" spans="2:12">
       <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
+        <v>115</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L39">
         <v>4000</v>
@@ -1458,36 +1461,39 @@
     </row>
     <row r="40" spans="2:12">
       <c r="K40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L40">
         <v>4020</v>
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="C41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
+      <c r="C41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L41">
         <v>4040</v>
@@ -1495,33 +1501,36 @@
     </row>
     <row r="42" spans="2:12">
       <c r="K42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L42">
         <v>4060</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="39">
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="G44" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="J44" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L44">
         <v>4100</v>
@@ -1530,7 +1539,7 @@
     <row r="45" spans="2:12">
       <c r="C45" s="5"/>
       <c r="K45" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L45">
         <v>4110</v>
@@ -1538,7 +1547,7 @@
     </row>
     <row r="46" spans="2:12">
       <c r="C46" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1547,13 +1556,13 @@
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L46">
         <v>4120</v>
@@ -1561,23 +1570,15 @@
     </row>
     <row r="47" spans="2:12">
       <c r="K47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L47">
         <v>4140</v>
       </c>
     </row>
-    <row r="48" spans="2:12">
-      <c r="K48" t="s">
-        <v>46</v>
-      </c>
-      <c r="L48">
-        <v>4160</v>
-      </c>
-    </row>
     <row r="49" spans="2:13">
       <c r="C49" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1586,16 +1587,16 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L49">
         <v>4180</v>
@@ -1603,7 +1604,7 @@
     </row>
     <row r="50" spans="2:13">
       <c r="K50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L50">
         <v>4200</v>
@@ -1611,16 +1612,16 @@
     </row>
     <row r="51" spans="2:13" ht="39">
       <c r="C51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L51">
         <v>4220</v>
@@ -1628,7 +1629,7 @@
     </row>
     <row r="52" spans="2:13">
       <c r="K52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L52">
         <v>4240</v>
@@ -1636,7 +1637,7 @@
     </row>
     <row r="53" spans="2:13">
       <c r="K53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L53">
         <v>4260</v>
@@ -1644,39 +1645,39 @@
     </row>
     <row r="54" spans="2:13">
       <c r="B54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>25</v>
-      </c>
-      <c r="I54" s="3" t="s">
+      <c r="J54" t="s">
         <v>124</v>
       </c>
-      <c r="J54" t="s">
-        <v>125</v>
-      </c>
       <c r="K54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L54">
         <v>4280</v>
       </c>
       <c r="M54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="2:13">
       <c r="K55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L55">
         <v>4300</v>
@@ -1684,27 +1685,27 @@
     </row>
     <row r="56" spans="2:13">
       <c r="C56" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L56">
         <v>4320</v>
       </c>
       <c r="M56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:13">
       <c r="K57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L57">
         <v>4340</v>
@@ -1712,19 +1713,19 @@
     </row>
     <row r="58" spans="2:13" ht="26">
       <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" t="s">
         <v>52</v>
       </c>
-      <c r="C58" t="s">
-        <v>53</v>
-      </c>
       <c r="I58" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J58" t="s">
         <v>58</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>59</v>
-      </c>
-      <c r="K58" t="s">
-        <v>60</v>
       </c>
       <c r="L58">
         <v>4360</v>
@@ -1732,7 +1733,7 @@
     </row>
     <row r="59" spans="2:13">
       <c r="K59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L59">
         <v>4380</v>
@@ -1740,16 +1741,16 @@
     </row>
     <row r="60" spans="2:13" ht="26">
       <c r="C60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I60" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K60" t="s">
         <v>75</v>
-      </c>
-      <c r="J60" t="s">
-        <v>45</v>
-      </c>
-      <c r="K60" t="s">
-        <v>76</v>
       </c>
       <c r="L60">
         <v>4400</v>
@@ -1757,7 +1758,7 @@
     </row>
     <row r="61" spans="2:13">
       <c r="K61" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L61">
         <v>4420</v>
@@ -1765,16 +1766,16 @@
     </row>
     <row r="62" spans="2:13">
       <c r="C62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I62" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J62" t="s">
         <v>77</v>
       </c>
-      <c r="J62" t="s">
-        <v>78</v>
-      </c>
       <c r="K62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L62">
         <v>4440</v>
@@ -1782,7 +1783,7 @@
     </row>
     <row r="63" spans="2:13">
       <c r="K63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L63">
         <v>4460</v>
@@ -1790,7 +1791,7 @@
     </row>
     <row r="64" spans="2:13">
       <c r="K64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L64">
         <v>4480</v>
@@ -1798,16 +1799,16 @@
     </row>
     <row r="65" spans="2:12" ht="26">
       <c r="C65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I65" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" t="s">
         <v>80</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>81</v>
-      </c>
-      <c r="K65" t="s">
-        <v>82</v>
       </c>
       <c r="L65">
         <v>4500</v>
@@ -1815,7 +1816,7 @@
     </row>
     <row r="66" spans="2:12">
       <c r="K66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L66">
         <v>4520</v>
@@ -1823,16 +1824,16 @@
     </row>
     <row r="67" spans="2:12">
       <c r="C67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L67">
         <v>4540</v>
@@ -1840,16 +1841,16 @@
     </row>
     <row r="68" spans="2:12" ht="26">
       <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="J68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L68">
         <v>4560</v>
@@ -1857,7 +1858,7 @@
     </row>
     <row r="69" spans="2:12">
       <c r="K69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L69">
         <v>4580</v>
@@ -1865,52 +1866,52 @@
     </row>
     <row r="70" spans="2:12">
       <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" t="s">
         <v>69</v>
       </c>
-      <c r="C70" t="s">
-        <v>70</v>
-      </c>
       <c r="G70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="2:12">
       <c r="C71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="2:12">
       <c r="C72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="2:12">
       <c r="C73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="2:12">
       <c r="B74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="2:12">
       <c r="B75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="2:12">
       <c r="B76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1942,10 +1943,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1953,7 +1954,7 @@
         <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1961,7 +1962,7 @@
         <v>317.31799999999998</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1969,7 +1970,7 @@
         <v>383</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1977,7 +1978,7 @@
         <v>384</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1985,7 +1986,7 @@
         <v>390</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added draft of new colection for reserved identifiers.  This needs to be discussed.
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -66,59 +66,59 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>UC06, UC09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierNotUnique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUID, systemMetadata, scienceMetadata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserveIdentifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC04, UC38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getLogRecords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC33</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>listObjects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>resolve</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC06, UC09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, GUID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierNotUnique</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GUID, systemMetadata, scienceMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>reserveIdentifier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC04, UC38</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getLogRecords</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC33</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>listObjects</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>create</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -960,8 +960,8 @@
   <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L48" sqref="L48"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1024,7 +1024,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
@@ -1042,7 +1042,7 @@
         <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
         <v>100</v>
@@ -1082,7 +1082,7 @@
         <v>29</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
         <v>104</v>
@@ -1352,7 +1352,7 @@
         <v>132</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>115</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="44" spans="2:12" ht="39">
       <c r="C44" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -1518,16 +1518,16 @@
         <v>1</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" t="s">
         <v>15</v>
-      </c>
-      <c r="J44" t="s">
-        <v>16</v>
       </c>
       <c r="K44" t="s">
         <v>46</v>
@@ -1539,20 +1539,23 @@
     <row r="45" spans="2:12">
       <c r="C45" s="5"/>
       <c r="K45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L45">
         <v>4110</v>
       </c>
     </row>
     <row r="46" spans="2:12">
-      <c r="C46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
+      <c r="C46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
@@ -1578,16 +1581,16 @@
     </row>
     <row r="49" spans="2:13">
       <c r="C49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
         <v>17</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="G49" t="s">
-        <v>18</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>40</v>
@@ -1657,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>123</v>
@@ -1685,7 +1688,7 @@
     </row>
     <row r="56" spans="2:13">
       <c r="C56" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
working through search attributes
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -22,10 +22,282 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
   <si>
+    <t>UC09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_control</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>replicate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC01, UC09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Scenario</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Funcational Use Case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID, accessLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, userid, GUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidtoken</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>username, password, authSystem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrincipalType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierNotUnique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>API</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Return</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exceptions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>errorDetail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_crud</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>describe</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getChecksum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getLogRecords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, GUID</t>
+  </si>
+  <si>
+    <t>token, GUID, [checksumAlgorithm]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, fromDate, toDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bytes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifierType</t>
+  </si>
+  <si>
+    <t>IdentifierType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DescribeResponse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemMetadata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checksum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LogRecords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>NotFound</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>IdentifierNotUnique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnsupportedType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsufficientResources</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvalidSystemMetadata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvalidRequest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_crud</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assertRelation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consistent mechanism for identifying users</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>typeOfOperation, targetGUID, requestorIdentity, dateOfRequest, ...</t>
+  </si>
+  <si>
+    <t>Recast parameters as query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotAuthorized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ObjectList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to work on query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to work on query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token, query</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_register</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_health</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN_synchronization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_authorization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_replication</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_capabilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN_health</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotFound</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>UC01, UC06</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -287,278 +559,6 @@
   </si>
   <si>
     <t>UC09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_control</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>replicate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC01, UC09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Scenario</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Funcational Use Case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>isAuthorized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, GUID, accessLevel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NotAuthorized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, userid, GUID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invalidtoken</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>username, password, authSystem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PrincipalType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierNotUnique</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Version</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>API</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Method</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parameters</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Return</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exceptions</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>errorDetail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN_crud</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>create</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>update</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>describe</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getChecksum</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getLogRecords</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, GUID</t>
-  </si>
-  <si>
-    <t>token, GUID, [checksumAlgorithm]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, fromDate, toDate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bytes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierType</t>
-  </si>
-  <si>
-    <t>IdentifierType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DescribeResponse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SystemMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checksum</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LogRecords</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NotAuthorized</t>
-  </si>
-  <si>
-    <t>NotAuthorized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NotFound</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifierNotUnique</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnsupportedType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InsufficientResources</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvalidSystemMetadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvalidRequest</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_crud</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>assertRelation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Consistent mechanism for identifying users</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>log</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>typeOfOperation, targetGUID, requestorIdentity, dateOfRequest, ...</t>
-  </si>
-  <si>
-    <t>Recast parameters as query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NotAuthorized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ObjectList</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Need to work on query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Need to work on query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>token, query</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_register</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_health</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN_synchronization</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN_authorization</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN_replication</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN_capabilities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN_health</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC01</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -961,7 +961,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -980,52 +980,52 @@
   <sheetData>
     <row r="1" spans="1:13" ht="61">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="7">
         <v>1</v>
       </c>
@@ -1036,19 +1036,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L2">
         <v>1000</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="K3" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>1020</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -1076,19 +1076,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L4">
         <v>1040</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="K5" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>1060</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="K6" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L6">
         <v>1080</v>
@@ -1112,19 +1112,19 @@
     </row>
     <row r="7" spans="1:13">
       <c r="C7" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L7">
         <v>1100</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="K8" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="L8">
         <v>1120</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="K9" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="L9">
         <v>1140</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="K10" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="L10">
         <v>1160</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="K11" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="L11">
         <v>1180</v>
@@ -1164,16 +1164,16 @@
     </row>
     <row r="12" spans="1:13">
       <c r="C12" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L12">
         <v>1200</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="K13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>1220</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="K14" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="L14">
         <v>1240</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="K15" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="L15">
         <v>1260</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="K16" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L16">
         <v>1280</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="K17" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="L17">
         <v>1300</v>
@@ -1221,16 +1221,16 @@
     </row>
     <row r="18" spans="2:13">
       <c r="C18" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L18">
         <v>1320</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="K19" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L19">
         <v>1340</v>
@@ -1246,16 +1246,16 @@
     </row>
     <row r="20" spans="2:13">
       <c r="C20" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="K20" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L20">
         <v>1360</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="K21" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L21">
         <v>1380</v>
@@ -1271,16 +1271,16 @@
     </row>
     <row r="22" spans="2:13" ht="26">
       <c r="C22" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="K22" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L22">
         <v>1400</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="K23" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L23">
         <v>1420</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="24" spans="2:13">
       <c r="K24" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="L24">
         <v>1440</v>
@@ -1304,27 +1304,27 @@
     </row>
     <row r="25" spans="2:13" ht="26">
       <c r="C25" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="K25" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L25">
         <v>1460</v>
       </c>
       <c r="M25" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="2:13">
       <c r="K26" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="L26">
         <v>1480</v>
@@ -1332,16 +1332,16 @@
     </row>
     <row r="27" spans="2:13" ht="52">
       <c r="C27" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L27">
         <v>1500</v>
@@ -1349,10 +1349,10 @@
     </row>
     <row r="28" spans="2:13" ht="52">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -1364,19 +1364,19 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="L28">
         <v>1520</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="K29" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L29">
         <v>1540</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="30" spans="2:13">
       <c r="K30" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="L30">
         <v>1560</v>
@@ -1400,36 +1400,36 @@
     </row>
     <row r="31" spans="2:13">
       <c r="C31" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="2:12">
       <c r="B33" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:12">
       <c r="B34" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:12">
       <c r="B35" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="K35" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="2:12">
       <c r="B39" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
@@ -1441,19 +1441,19 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="J39" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="K39" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L39">
         <v>4000</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="40" spans="2:12">
       <c r="K40" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L40">
         <v>4020</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="41" spans="2:12">
       <c r="C41" s="7" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
@@ -1481,19 +1481,19 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="H41" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="J41" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="K41" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L41">
         <v>4040</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="42" spans="2:12">
       <c r="K42" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L42">
         <v>4060</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="44" spans="2:12" ht="39">
       <c r="C44" s="7" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -1518,19 +1518,19 @@
         <v>1</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="J44" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="K44" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="L44">
         <v>4100</v>
@@ -1539,7 +1539,7 @@
     <row r="45" spans="2:12">
       <c r="C45" s="5"/>
       <c r="K45" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="L45">
         <v>4110</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="46" spans="2:12">
       <c r="C46" s="7" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="D46" s="7">
         <v>1</v>
@@ -1559,13 +1559,13 @@
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="J46" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="K46" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L46">
         <v>4120</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="47" spans="2:12">
       <c r="K47" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L47">
         <v>4140</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="49" spans="2:13">
       <c r="C49" s="5" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1590,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="J49" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="K49" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L49">
         <v>4180</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="50" spans="2:13">
       <c r="K50" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L50">
         <v>4200</v>
@@ -1615,16 +1615,16 @@
     </row>
     <row r="51" spans="2:13" ht="39">
       <c r="C51" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="I51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J51" t="s">
+        <v>113</v>
+      </c>
+      <c r="K51" t="s">
         <v>41</v>
-      </c>
-      <c r="J51" t="s">
-        <v>44</v>
-      </c>
-      <c r="K51" t="s">
-        <v>108</v>
       </c>
       <c r="L51">
         <v>4220</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="52" spans="2:13">
       <c r="K52" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L52">
         <v>4240</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="53" spans="2:13">
       <c r="K53" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="L53">
         <v>4260</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="54" spans="2:13">
       <c r="B54" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1659,28 +1659,31 @@
       <c r="E54">
         <v>1</v>
       </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="J54" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="K54" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L54">
         <v>4280</v>
       </c>
       <c r="M54" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="2:13">
       <c r="K55" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L55">
         <v>4300</v>
@@ -1688,27 +1691,27 @@
     </row>
     <row r="56" spans="2:13">
       <c r="C56" s="5" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="J56" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="K56" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L56">
         <v>4320</v>
       </c>
       <c r="M56" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="2:13">
       <c r="K57" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="L57">
         <v>4340</v>
@@ -1716,19 +1719,19 @@
     </row>
     <row r="58" spans="2:13" ht="26">
       <c r="B58" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="J58" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="K58" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="L58">
         <v>4360</v>
@@ -1736,7 +1739,7 @@
     </row>
     <row r="59" spans="2:13">
       <c r="K59" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="L59">
         <v>4380</v>
@@ -1744,16 +1747,16 @@
     </row>
     <row r="60" spans="2:13" ht="26">
       <c r="C60" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="J60" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="K60" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="L60">
         <v>4400</v>
@@ -1761,7 +1764,7 @@
     </row>
     <row r="61" spans="2:13">
       <c r="K61" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L61">
         <v>4420</v>
@@ -1769,16 +1772,16 @@
     </row>
     <row r="62" spans="2:13">
       <c r="C62" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="J62" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="K62" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="L62">
         <v>4440</v>
@@ -1786,7 +1789,7 @@
     </row>
     <row r="63" spans="2:13">
       <c r="K63" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L63">
         <v>4460</v>
@@ -1794,7 +1797,7 @@
     </row>
     <row r="64" spans="2:13">
       <c r="K64" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="L64">
         <v>4480</v>
@@ -1802,16 +1805,16 @@
     </row>
     <row r="65" spans="2:12" ht="26">
       <c r="C65" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="J65" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="K65" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="L65">
         <v>4500</v>
@@ -1819,7 +1822,7 @@
     </row>
     <row r="66" spans="2:12">
       <c r="K66" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="L66">
         <v>4520</v>
@@ -1827,16 +1830,16 @@
     </row>
     <row r="67" spans="2:12">
       <c r="C67" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="K67" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="L67">
         <v>4540</v>
@@ -1844,16 +1847,16 @@
     </row>
     <row r="68" spans="2:12" ht="26">
       <c r="C68" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="J68" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="K68" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="L68">
         <v>4560</v>
@@ -1861,7 +1864,7 @@
     </row>
     <row r="69" spans="2:12">
       <c r="K69" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="L69">
         <v>4580</v>
@@ -1869,58 +1872,57 @@
     </row>
     <row r="70" spans="2:12">
       <c r="B70" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="G70" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:12">
       <c r="C71" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="G71" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="2:12">
       <c r="C72" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="G72" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="2:12">
       <c r="C73" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="G73" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:12">
       <c r="B74" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="2:12">
       <c r="B75" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="2:12">
       <c r="B76" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1946,10 +1948,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1957,7 +1959,7 @@
         <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1965,7 +1967,7 @@
         <v>317.31799999999998</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1973,7 +1975,7 @@
         <v>383</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1981,7 +1983,7 @@
         <v>384</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1989,7 +1991,7 @@
         <v>390</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added detail codes for ServiceFailure in method cross refernece spreadsheet
</commit_message>
<xml_diff>
--- a/MethodCrossReference.xlsx
+++ b/MethodCrossReference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="-100" windowWidth="26340" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="4180" yWindow="1660" windowWidth="26920" windowHeight="17720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MethodMadnessMap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
+  <si>
+    <t>SystemFailure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>UC09</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -957,11 +961,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -980,51 +984,51 @@
   <sheetData>
     <row r="1" spans="1:13" ht="61">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
@@ -1036,19 +1040,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>1000</v>
@@ -1056,873 +1060,1078 @@
     </row>
     <row r="3" spans="1:13">
       <c r="K3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>1020</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="C4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
-      </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1040</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="5" spans="1:13">
+      <c r="C5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
       <c r="K5" t="s">
         <v>42</v>
       </c>
       <c r="L5">
-        <v>1060</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="K6" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="L6">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="K7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7">
         <v>1080</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7">
-        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="K8" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1120</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="9" spans="1:13">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L9">
-        <v>1140</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L10">
-        <v>1160</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="K11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="K12" t="s">
         <v>46</v>
       </c>
-      <c r="L11">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
-      </c>
       <c r="L12">
-        <v>1200</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="K13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L13">
-        <v>1220</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="K14" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>1240</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="15" spans="1:13">
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
       <c r="K15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L15">
-        <v>1260</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="K16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L16">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13">
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
+      <c r="K18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19">
         <v>1280</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
-      <c r="K17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L17">
+    <row r="20" spans="3:13">
+      <c r="K20" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20">
         <v>1300</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="K19" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="C20" t="s">
+    <row r="21" spans="3:13">
+      <c r="K21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
+      <c r="C22" t="s">
         <v>27</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J20" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" t="s">
-        <v>41</v>
-      </c>
-      <c r="L20">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13">
-      <c r="K21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L21">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="26">
-      <c r="C22" t="s">
-        <v>28</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="J22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L22">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
+      <c r="K24" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13">
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13">
+      <c r="K26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13">
+      <c r="K27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" ht="26">
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28">
         <v>1400</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
-      <c r="K23" t="s">
+    <row r="29" spans="3:13">
+      <c r="K29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
+      <c r="K30" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13">
+      <c r="K31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" ht="26">
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" t="s">
         <v>42</v>
       </c>
-      <c r="L23">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13">
-      <c r="K24" t="s">
-        <v>47</v>
-      </c>
-      <c r="L24">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="26">
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" t="s">
-        <v>41</v>
-      </c>
-      <c r="L25">
+      <c r="L32">
         <v>1460</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="K33" t="s">
+        <v>48</v>
+      </c>
+      <c r="L33">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="K34" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="52">
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="2:13">
-      <c r="K26" t="s">
-        <v>47</v>
-      </c>
-      <c r="L26">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" ht="52">
-      <c r="C27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K27" t="s">
-        <v>114</v>
-      </c>
-      <c r="L27">
+      <c r="K35" t="s">
+        <v>115</v>
+      </c>
+      <c r="L35">
         <v>1500</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="52">
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="E28" s="7">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I28" s="3" t="s">
+    <row r="36" spans="2:12">
+      <c r="K36" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="52">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" t="s">
+        <v>103</v>
+      </c>
+      <c r="K37" t="s">
+        <v>104</v>
+      </c>
+      <c r="L37">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="K38" t="s">
+        <v>115</v>
+      </c>
+      <c r="L38">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="K39" t="s">
         <v>78</v>
       </c>
-      <c r="J28" t="s">
-        <v>102</v>
-      </c>
-      <c r="K28" t="s">
-        <v>103</v>
-      </c>
-      <c r="L28">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13">
-      <c r="K29" t="s">
-        <v>114</v>
-      </c>
-      <c r="L29">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
-      <c r="K30" t="s">
-        <v>77</v>
-      </c>
-      <c r="L30">
+      <c r="L39">
         <v>1560</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13">
-      <c r="C31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12">
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12">
-      <c r="B34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12">
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="K35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="7">
-        <v>1</v>
-      </c>
-      <c r="E39" s="7">
-        <v>1</v>
-      </c>
-      <c r="F39" s="7">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H39" t="s">
-        <v>100</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J39" t="s">
-        <v>33</v>
-      </c>
-      <c r="K39" t="s">
-        <v>41</v>
-      </c>
-      <c r="L39">
-        <v>4000</v>
       </c>
     </row>
     <row r="40" spans="2:12">
       <c r="K40" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>4020</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="C41" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="7">
-        <v>1</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" t="s">
-        <v>99</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J41" t="s">
-        <v>37</v>
-      </c>
-      <c r="K41" t="s">
-        <v>41</v>
-      </c>
-      <c r="L41">
-        <v>4040</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12">
-      <c r="K42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L42">
-        <v>4060</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="39">
-      <c r="C44" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="7">
-        <v>1</v>
-      </c>
-      <c r="E44" s="7">
-        <v>1</v>
-      </c>
-      <c r="F44" s="7" t="s">
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" t="s">
+        <v>70</v>
+      </c>
+      <c r="L45">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="K46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G44" t="s">
-        <v>80</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J44" t="s">
-        <v>84</v>
-      </c>
-      <c r="K44" t="s">
-        <v>115</v>
-      </c>
-      <c r="L44">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12">
-      <c r="C45" s="5"/>
-      <c r="K45" t="s">
-        <v>82</v>
-      </c>
-      <c r="L45">
-        <v>4110</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12">
-      <c r="C46" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="7">
-        <v>1</v>
-      </c>
-      <c r="E46" s="7">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7">
-        <v>1</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J46" t="s">
-        <v>111</v>
-      </c>
-      <c r="K46" t="s">
-        <v>41</v>
-      </c>
-      <c r="L46">
-        <v>4120</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12">
-      <c r="K47" t="s">
-        <v>42</v>
-      </c>
-      <c r="L47">
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13">
-      <c r="C49" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
+      <c r="D49" s="7">
+        <v>1</v>
+      </c>
+      <c r="E49" s="7">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="H49" t="s">
+        <v>101</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>109</v>
       </c>
       <c r="J49" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="K49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L49">
-        <v>4180</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12">
       <c r="K50" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="L50">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" ht="39">
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J51" t="s">
-        <v>113</v>
-      </c>
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12">
       <c r="K51" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="L51">
-        <v>4220</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="C52" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="7">
+        <v>1</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" t="s">
+        <v>100</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" t="s">
+        <v>38</v>
+      </c>
       <c r="K52" t="s">
         <v>42</v>
       </c>
       <c r="L52">
-        <v>4240</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12">
       <c r="K53" t="s">
+        <v>43</v>
+      </c>
+      <c r="L53">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="K54" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="39">
+      <c r="C55" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="7">
+        <v>1</v>
+      </c>
+      <c r="E55" s="7">
+        <v>1</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" t="s">
+        <v>81</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J55" t="s">
+        <v>85</v>
+      </c>
+      <c r="K55" t="s">
         <v>116</v>
       </c>
-      <c r="L53">
-        <v>4260</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13">
-      <c r="B54" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>88</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J54" t="s">
-        <v>57</v>
-      </c>
-      <c r="K54" t="s">
-        <v>41</v>
-      </c>
-      <c r="L54">
-        <v>4280</v>
-      </c>
-      <c r="M54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13">
-      <c r="K55" t="s">
-        <v>114</v>
-      </c>
       <c r="L55">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13">
-      <c r="C56" s="5" t="s">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12">
+      <c r="C56" s="5"/>
+      <c r="K56" t="s">
+        <v>83</v>
+      </c>
+      <c r="L56">
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12">
+      <c r="C57" s="5"/>
+      <c r="K57" t="s">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>4115</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="C58" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="7">
+        <v>1</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7">
+        <v>1</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J58" t="s">
+        <v>112</v>
+      </c>
+      <c r="K58" t="s">
+        <v>42</v>
+      </c>
+      <c r="L58">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="K59" t="s">
+        <v>43</v>
+      </c>
+      <c r="L59">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="K60" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12">
+      <c r="C61" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
         <v>87</v>
       </c>
-      <c r="I56" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J56" t="s">
-        <v>39</v>
-      </c>
-      <c r="K56" t="s">
-        <v>41</v>
-      </c>
-      <c r="L56">
-        <v>4320</v>
-      </c>
-      <c r="M56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13">
-      <c r="K57" t="s">
-        <v>114</v>
-      </c>
-      <c r="L57">
-        <v>4340</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" ht="26">
-      <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" t="s">
-        <v>121</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J58" t="s">
-        <v>127</v>
-      </c>
-      <c r="K58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L58">
-        <v>4360</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13">
-      <c r="K59" t="s">
-        <v>129</v>
-      </c>
-      <c r="L59">
-        <v>4380</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" ht="26">
-      <c r="C60" t="s">
-        <v>122</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J60" t="s">
+      <c r="I61" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J61" t="s">
         <v>113</v>
       </c>
-      <c r="K60" t="s">
-        <v>8</v>
-      </c>
-      <c r="L60">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13">
       <c r="K61" t="s">
         <v>42</v>
       </c>
       <c r="L61">
-        <v>4420</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13">
-      <c r="C62" t="s">
-        <v>123</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J62" t="s">
-        <v>10</v>
-      </c>
+        <v>4180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12">
       <c r="K62" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="L62">
-        <v>4440</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12">
       <c r="K63" t="s">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="39">
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J64" t="s">
+        <v>114</v>
+      </c>
+      <c r="K64" t="s">
         <v>42</v>
       </c>
-      <c r="L63">
-        <v>4460</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13">
-      <c r="K64" t="s">
-        <v>11</v>
-      </c>
       <c r="L64">
-        <v>4480</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" ht="26">
-      <c r="C65" t="s">
-        <v>124</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J65" t="s">
-        <v>13</v>
-      </c>
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13">
       <c r="K65" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="L65">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13">
       <c r="K66" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="L66">
-        <v>4520</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12">
-      <c r="C67" t="s">
-        <v>125</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J67" t="s">
-        <v>113</v>
-      </c>
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13">
       <c r="K67" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="L67">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" ht="26">
-      <c r="C68" t="s">
-        <v>94</v>
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13">
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="s">
+        <v>89</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="J68" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="K68" t="s">
         <v>42</v>
       </c>
       <c r="L68">
+        <v>4280</v>
+      </c>
+      <c r="M68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13">
+      <c r="K69" t="s">
+        <v>115</v>
+      </c>
+      <c r="L69">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13">
+      <c r="K70" t="s">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13">
+      <c r="C71" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J71" t="s">
+        <v>40</v>
+      </c>
+      <c r="K71" t="s">
+        <v>42</v>
+      </c>
+      <c r="L71">
+        <v>4320</v>
+      </c>
+      <c r="M71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13">
+      <c r="K72" t="s">
+        <v>115</v>
+      </c>
+      <c r="L72">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13">
+      <c r="K73" t="s">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" ht="26">
+      <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" t="s">
+        <v>122</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J74" t="s">
+        <v>128</v>
+      </c>
+      <c r="K74" t="s">
+        <v>129</v>
+      </c>
+      <c r="L74">
+        <v>4360</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13">
+      <c r="K75" t="s">
+        <v>130</v>
+      </c>
+      <c r="L75">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13">
+      <c r="K76" t="s">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" ht="26">
+      <c r="C77" t="s">
+        <v>123</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J77" t="s">
+        <v>114</v>
+      </c>
+      <c r="K77" t="s">
+        <v>9</v>
+      </c>
+      <c r="L77">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13">
+      <c r="K78" t="s">
+        <v>43</v>
+      </c>
+      <c r="L78">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13">
+      <c r="K79" t="s">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13">
+      <c r="C80" t="s">
+        <v>124</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J80" t="s">
+        <v>11</v>
+      </c>
+      <c r="K80" t="s">
+        <v>42</v>
+      </c>
+      <c r="L80">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="K81" t="s">
+        <v>43</v>
+      </c>
+      <c r="L81">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="K82" t="s">
+        <v>12</v>
+      </c>
+      <c r="L82">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="K83" t="s">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" ht="26">
+      <c r="C84" t="s">
+        <v>125</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J84" t="s">
+        <v>14</v>
+      </c>
+      <c r="K84" t="s">
+        <v>15</v>
+      </c>
+      <c r="L84">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="K85" t="s">
+        <v>129</v>
+      </c>
+      <c r="L85">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="K86" t="s">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12">
+      <c r="C87" t="s">
+        <v>126</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J87" t="s">
+        <v>114</v>
+      </c>
+      <c r="K87" t="s">
+        <v>55</v>
+      </c>
+      <c r="L87">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="K88" t="s">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" ht="26">
+      <c r="C89" t="s">
+        <v>95</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J89" t="s">
+        <v>114</v>
+      </c>
+      <c r="K89" t="s">
+        <v>43</v>
+      </c>
+      <c r="L89">
         <v>4560</v>
       </c>
     </row>
-    <row r="69" spans="2:12">
-      <c r="K69" t="s">
-        <v>40</v>
-      </c>
-      <c r="L69">
+    <row r="90" spans="2:12">
+      <c r="K90" t="s">
+        <v>41</v>
+      </c>
+      <c r="L90">
         <v>4580</v>
       </c>
     </row>
-    <row r="70" spans="2:12">
-      <c r="B70" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
+    <row r="91" spans="2:12">
+      <c r="K91" t="s">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12">
+      <c r="B92" t="s">
         <v>2</v>
       </c>
-      <c r="G70" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12">
-      <c r="C71" t="s">
-        <v>132</v>
-      </c>
-      <c r="G71" t="s">
+      <c r="C92" t="s">
+        <v>3</v>
+      </c>
+      <c r="G92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12">
+      <c r="C93" t="s">
+        <v>133</v>
+      </c>
+      <c r="G93" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12">
+      <c r="C94" t="s">
+        <v>134</v>
+      </c>
+      <c r="G94" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12">
+      <c r="C95" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="72" spans="2:12">
-      <c r="C72" t="s">
-        <v>133</v>
-      </c>
-      <c r="G72" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12">
-      <c r="C73" t="s">
-        <v>134</v>
-      </c>
-      <c r="G73" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12">
-      <c r="B74" t="s">
+      <c r="G95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12">
+      <c r="B96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12">
-      <c r="B75" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12">
-      <c r="B76" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1948,10 +2157,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1959,7 +2168,7 @@
         <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1967,7 +2176,7 @@
         <v>317.31799999999998</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1975,7 +2184,7 @@
         <v>383</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1983,7 +2192,7 @@
         <v>384</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1991,7 +2200,7 @@
         <v>390</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>